<commit_message>
adding hudson dataset to nutrient tests
</commit_message>
<xml_diff>
--- a/Prototypes/Nutrient/observed.xlsx
+++ b/Prototypes/Nutrient/observed.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2679" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2701" uniqueCount="58">
   <si>
     <t>SimulationName</t>
   </si>
@@ -194,13 +194,20 @@
   <si>
     <t>TON0_30cm</t>
   </si>
+  <si>
+    <t>W1</t>
+  </si>
+  <si>
+    <t>HudsonW1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -231,10 +238,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -16260,18 +16268,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N199"/>
+  <dimension ref="A1:N210"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="576" topLeftCell="A124" activePane="bottomLeft"/>
+      <pane ySplit="576" topLeftCell="A175" activePane="bottomLeft"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="K129" sqref="K129"/>
+      <selection pane="bottomLeft" activeCell="A200" sqref="A200:A210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -21845,6 +21854,160 @@
         <v>9.6199261992619931</v>
       </c>
     </row>
+    <row r="200" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>57</v>
+      </c>
+      <c r="B200" t="s">
+        <v>56</v>
+      </c>
+      <c r="F200" s="3">
+        <v>34574</v>
+      </c>
+      <c r="G200">
+        <v>14546.1538461538</v>
+      </c>
+    </row>
+    <row r="201" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
+        <v>57</v>
+      </c>
+      <c r="B201" t="s">
+        <v>56</v>
+      </c>
+      <c r="F201" s="3">
+        <v>34999</v>
+      </c>
+      <c r="G201">
+        <v>14499.9999999999</v>
+      </c>
+    </row>
+    <row r="202" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>57</v>
+      </c>
+      <c r="B202" t="s">
+        <v>56</v>
+      </c>
+      <c r="F202" s="3">
+        <v>35152</v>
+      </c>
+      <c r="G202">
+        <v>14996.1538461538</v>
+      </c>
+    </row>
+    <row r="203" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
+        <v>57</v>
+      </c>
+      <c r="B203" t="s">
+        <v>56</v>
+      </c>
+      <c r="F203" s="3">
+        <v>35361</v>
+      </c>
+      <c r="G203">
+        <v>14315.384615384601</v>
+      </c>
+    </row>
+    <row r="204" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
+        <v>57</v>
+      </c>
+      <c r="B204" t="s">
+        <v>56</v>
+      </c>
+      <c r="F204" s="3">
+        <v>35514</v>
+      </c>
+      <c r="G204">
+        <v>14765.384615384599</v>
+      </c>
+    </row>
+    <row r="205" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
+        <v>57</v>
+      </c>
+      <c r="B205" t="s">
+        <v>56</v>
+      </c>
+      <c r="F205" s="3">
+        <v>35729</v>
+      </c>
+      <c r="G205">
+        <v>14511.538461538401</v>
+      </c>
+    </row>
+    <row r="206" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
+        <v>57</v>
+      </c>
+      <c r="B206" t="s">
+        <v>56</v>
+      </c>
+      <c r="F206" s="3">
+        <v>35910</v>
+      </c>
+      <c r="G206">
+        <v>15261.538461538401</v>
+      </c>
+    </row>
+    <row r="207" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
+        <v>57</v>
+      </c>
+      <c r="B207" t="s">
+        <v>56</v>
+      </c>
+      <c r="F207" s="3">
+        <v>36093</v>
+      </c>
+      <c r="G207">
+        <v>14753.8461538461</v>
+      </c>
+    </row>
+    <row r="208" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
+        <v>57</v>
+      </c>
+      <c r="B208" t="s">
+        <v>56</v>
+      </c>
+      <c r="F208" s="3">
+        <v>36307</v>
+      </c>
+      <c r="G208">
+        <v>15250</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A209" t="s">
+        <v>57</v>
+      </c>
+      <c r="B209" t="s">
+        <v>56</v>
+      </c>
+      <c r="F209" s="3">
+        <v>36461</v>
+      </c>
+      <c r="G209">
+        <v>14730.7692307692</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>57</v>
+      </c>
+      <c r="B210" t="s">
+        <v>56</v>
+      </c>
+      <c r="F210" s="3">
+        <v>36642</v>
+      </c>
+      <c r="G210">
+        <v>14523.0769230769</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding BCS to nutrient validation
</commit_message>
<xml_diff>
--- a/Prototypes/Nutrient/observed.xlsx
+++ b/Prototypes/Nutrient/observed.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2701" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2748" uniqueCount="63">
   <si>
     <t>SimulationName</t>
   </si>
@@ -200,6 +200,21 @@
   <si>
     <t>HudsonW1</t>
   </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>HudsonP3</t>
+  </si>
+  <si>
+    <t>Brigalow</t>
+  </si>
+  <si>
+    <t>CropUpper</t>
+  </si>
+  <si>
+    <t>TON0_10cm</t>
+  </si>
 </sst>
 </file>
 
@@ -238,11 +253,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -16268,12 +16284,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N210"/>
+  <dimension ref="A1:O233"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="576" topLeftCell="A175" activePane="bottomLeft"/>
+      <pane ySplit="576" topLeftCell="A190" activePane="bottomLeft"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="A200" sqref="A200:A210"/>
+      <selection pane="bottomLeft" activeCell="A222" sqref="A222:B233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16281,10 +16297,10 @@
     <col min="1" max="1" width="37.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -16316,19 +16332,22 @@
         <v>33</v>
       </c>
       <c r="K1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" t="s">
         <v>55</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>52</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>53</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -16345,7 +16364,7 @@
         <v>28855</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -16374,7 +16393,7 @@
         <v>33806</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -16403,7 +16422,7 @@
         <v>35163</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -16432,7 +16451,7 @@
         <v>36575</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -16461,7 +16480,7 @@
         <v>34640</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -16490,7 +16509,7 @@
         <v>27549</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -16519,7 +16538,7 @@
         <v>30536</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -16548,7 +16567,7 @@
         <v>28344</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -16577,7 +16596,7 @@
         <v>32624</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -16606,7 +16625,7 @@
         <v>28935</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -16635,7 +16654,7 @@
         <v>27190</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -16664,7 +16683,7 @@
         <v>27960</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -16681,7 +16700,7 @@
         <v>28855</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -16698,7 +16717,7 @@
         <v>29220</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -20151,7 +20170,7 @@
         <v>35140</v>
       </c>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>23</v>
       </c>
@@ -20180,7 +20199,7 @@
         <v>30910</v>
       </c>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>38</v>
       </c>
@@ -20196,22 +20215,22 @@
       <c r="J146">
         <v>48670</v>
       </c>
-      <c r="K146">
+      <c r="L146">
         <v>3710</v>
       </c>
-      <c r="L146">
+      <c r="M146">
         <v>2880</v>
       </c>
-      <c r="M146">
-        <f>J146/K146</f>
+      <c r="N146">
+        <f>J146/L146</f>
         <v>13.118598382749326</v>
       </c>
-      <c r="N146">
-        <f>I146/L146</f>
+      <c r="O146">
+        <f>I146/M146</f>
         <v>11.635416666666666</v>
       </c>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>51</v>
       </c>
@@ -20227,22 +20246,22 @@
       <c r="J147">
         <v>48120</v>
       </c>
-      <c r="K147">
+      <c r="L147">
         <v>3660</v>
       </c>
-      <c r="L147">
+      <c r="M147">
         <v>2960</v>
       </c>
-      <c r="M147">
-        <f t="shared" ref="M147:M199" si="0">J147/K147</f>
+      <c r="N147">
+        <f t="shared" ref="N147:N199" si="0">J147/L147</f>
         <v>13.147540983606557</v>
       </c>
-      <c r="N147">
-        <f t="shared" ref="N147:N199" si="1">I147/L147</f>
+      <c r="O147">
+        <f t="shared" ref="O147:O199" si="1">I147/M147</f>
         <v>11.641891891891891</v>
       </c>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>34</v>
       </c>
@@ -20258,22 +20277,22 @@
       <c r="J148">
         <v>49240</v>
       </c>
-      <c r="K148">
+      <c r="L148">
         <v>3750</v>
       </c>
-      <c r="L148">
+      <c r="M148">
         <v>2990</v>
       </c>
-      <c r="M148">
+      <c r="N148">
         <f t="shared" si="0"/>
         <v>13.130666666666666</v>
       </c>
-      <c r="N148">
+      <c r="O148">
         <f t="shared" si="1"/>
         <v>11.662207357859531</v>
       </c>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>35</v>
       </c>
@@ -20289,22 +20308,22 @@
       <c r="J149">
         <v>49410</v>
       </c>
-      <c r="K149">
+      <c r="L149">
         <v>3770</v>
       </c>
-      <c r="L149">
+      <c r="M149">
         <v>3050</v>
       </c>
-      <c r="M149">
+      <c r="N149">
         <f t="shared" si="0"/>
         <v>13.106100795755967</v>
       </c>
-      <c r="N149">
+      <c r="O149">
         <f t="shared" si="1"/>
         <v>11.672131147540984</v>
       </c>
     </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>40</v>
       </c>
@@ -20320,22 +20339,22 @@
       <c r="J150">
         <v>48570</v>
       </c>
-      <c r="K150">
+      <c r="L150">
         <v>3730</v>
       </c>
-      <c r="L150">
+      <c r="M150">
         <v>2900</v>
       </c>
-      <c r="M150">
+      <c r="N150">
         <f t="shared" si="0"/>
         <v>13.021447721179625</v>
       </c>
-      <c r="N150">
+      <c r="O150">
         <f t="shared" si="1"/>
         <v>11.644827586206896</v>
       </c>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>42</v>
       </c>
@@ -20351,22 +20370,22 @@
       <c r="J151">
         <v>50210</v>
       </c>
-      <c r="K151">
+      <c r="L151">
         <v>3830</v>
       </c>
-      <c r="L151">
+      <c r="M151">
         <v>3150</v>
       </c>
-      <c r="M151">
+      <c r="N151">
         <f t="shared" si="0"/>
         <v>13.109660574412533</v>
       </c>
-      <c r="N151">
+      <c r="O151">
         <f t="shared" si="1"/>
         <v>11.641269841269841</v>
       </c>
     </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>36</v>
       </c>
@@ -20382,22 +20401,22 @@
       <c r="J152">
         <v>49900</v>
       </c>
-      <c r="K152">
+      <c r="L152">
         <v>3810</v>
       </c>
-      <c r="L152">
+      <c r="M152">
         <v>3100</v>
       </c>
-      <c r="M152">
+      <c r="N152">
         <f t="shared" si="0"/>
         <v>13.097112860892388</v>
       </c>
-      <c r="N152">
+      <c r="O152">
         <f t="shared" si="1"/>
         <v>11.651612903225807</v>
       </c>
     </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>37</v>
       </c>
@@ -20413,22 +20432,22 @@
       <c r="J153">
         <v>48750</v>
       </c>
-      <c r="K153">
+      <c r="L153">
         <v>3710</v>
       </c>
-      <c r="L153">
+      <c r="M153">
         <v>3040</v>
       </c>
-      <c r="M153">
+      <c r="N153">
         <f t="shared" si="0"/>
         <v>13.140161725067385</v>
       </c>
-      <c r="N153">
+      <c r="O153">
         <f t="shared" si="1"/>
         <v>11.674342105263158</v>
       </c>
     </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>41</v>
       </c>
@@ -20444,22 +20463,22 @@
       <c r="J154">
         <v>49920</v>
       </c>
-      <c r="K154">
+      <c r="L154">
         <v>3810</v>
       </c>
-      <c r="L154">
+      <c r="M154">
         <v>3100</v>
       </c>
-      <c r="M154">
+      <c r="N154">
         <f t="shared" si="0"/>
         <v>13.102362204724409</v>
       </c>
-      <c r="N154">
+      <c r="O154">
         <f t="shared" si="1"/>
         <v>11.648387096774194</v>
       </c>
     </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>38</v>
       </c>
@@ -20475,22 +20494,22 @@
       <c r="J155">
         <v>46440</v>
       </c>
-      <c r="K155">
+      <c r="L155">
         <v>3560</v>
       </c>
-      <c r="L155">
+      <c r="M155">
         <v>2970</v>
       </c>
-      <c r="M155">
+      <c r="N155">
         <f t="shared" si="0"/>
         <v>13.044943820224718</v>
       </c>
-      <c r="N155">
+      <c r="O155">
         <f t="shared" si="1"/>
         <v>11.437710437710438</v>
       </c>
     </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>51</v>
       </c>
@@ -20506,22 +20525,22 @@
       <c r="J156">
         <v>45740</v>
       </c>
-      <c r="K156">
+      <c r="L156">
         <v>3510</v>
       </c>
-      <c r="L156">
+      <c r="M156">
         <v>2950</v>
       </c>
-      <c r="M156">
+      <c r="N156">
         <f t="shared" si="0"/>
         <v>13.031339031339032</v>
       </c>
-      <c r="N156">
+      <c r="O156">
         <f t="shared" si="1"/>
         <v>11.427118644067797</v>
       </c>
     </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>34</v>
       </c>
@@ -20537,22 +20556,22 @@
       <c r="J157">
         <v>48080</v>
       </c>
-      <c r="K157">
+      <c r="L157">
         <v>3690</v>
       </c>
-      <c r="L157">
+      <c r="M157">
         <v>2890</v>
       </c>
-      <c r="M157">
+      <c r="N157">
         <f t="shared" si="0"/>
         <v>13.029810298102982</v>
       </c>
-      <c r="N157">
+      <c r="O157">
         <f t="shared" si="1"/>
         <v>11.453287197231834</v>
       </c>
     </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>35</v>
       </c>
@@ -20568,22 +20587,22 @@
       <c r="J158">
         <v>47080</v>
       </c>
-      <c r="K158">
+      <c r="L158">
         <v>3610</v>
       </c>
-      <c r="L158">
+      <c r="M158">
         <v>2890</v>
       </c>
-      <c r="M158">
+      <c r="N158">
         <f t="shared" si="0"/>
         <v>13.041551246537397</v>
       </c>
-      <c r="N158">
+      <c r="O158">
         <f t="shared" si="1"/>
         <v>11.446366782006921</v>
       </c>
     </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>40</v>
       </c>
@@ -20599,22 +20618,22 @@
       <c r="J159">
         <v>50880</v>
       </c>
-      <c r="K159">
+      <c r="L159">
         <v>3900</v>
       </c>
-      <c r="L159">
+      <c r="M159">
         <v>2820</v>
       </c>
-      <c r="M159">
+      <c r="N159">
         <f t="shared" si="0"/>
         <v>13.046153846153846</v>
       </c>
-      <c r="N159">
+      <c r="O159">
         <f t="shared" si="1"/>
         <v>11.439716312056737</v>
       </c>
     </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>42</v>
       </c>
@@ -20630,22 +20649,22 @@
       <c r="J160">
         <v>49230</v>
       </c>
-      <c r="K160">
+      <c r="L160">
         <v>3780</v>
       </c>
-      <c r="L160">
+      <c r="M160">
         <v>3120</v>
       </c>
-      <c r="M160">
+      <c r="N160">
         <f t="shared" si="0"/>
         <v>13.023809523809524</v>
       </c>
-      <c r="N160">
+      <c r="O160">
         <f t="shared" si="1"/>
         <v>11.435897435897436</v>
       </c>
     </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>36</v>
       </c>
@@ -20661,22 +20680,22 @@
       <c r="J161">
         <v>48360</v>
       </c>
-      <c r="K161">
+      <c r="L161">
         <v>3710</v>
       </c>
-      <c r="L161">
+      <c r="M161">
         <v>2980</v>
       </c>
-      <c r="M161">
+      <c r="N161">
         <f t="shared" si="0"/>
         <v>13.035040431266847</v>
       </c>
-      <c r="N161">
+      <c r="O161">
         <f t="shared" si="1"/>
         <v>11.466442953020135</v>
       </c>
     </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>37</v>
       </c>
@@ -20692,22 +20711,22 @@
       <c r="J162">
         <v>48590</v>
       </c>
-      <c r="K162">
+      <c r="L162">
         <v>3720</v>
       </c>
-      <c r="L162">
+      <c r="M162">
         <v>2880</v>
       </c>
-      <c r="M162">
+      <c r="N162">
         <f t="shared" si="0"/>
         <v>13.061827956989248</v>
       </c>
-      <c r="N162">
+      <c r="O162">
         <f t="shared" si="1"/>
         <v>11.430555555555555</v>
       </c>
     </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>41</v>
       </c>
@@ -20723,22 +20742,22 @@
       <c r="J163">
         <v>50480</v>
       </c>
-      <c r="K163">
+      <c r="L163">
         <v>3870</v>
       </c>
-      <c r="L163">
+      <c r="M163">
         <v>2960</v>
       </c>
-      <c r="M163">
+      <c r="N163">
         <f t="shared" si="0"/>
         <v>13.043927648578812</v>
       </c>
-      <c r="N163">
+      <c r="O163">
         <f t="shared" si="1"/>
         <v>11.462837837837839</v>
       </c>
     </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>38</v>
       </c>
@@ -20754,22 +20773,22 @@
       <c r="J164">
         <v>42150</v>
       </c>
-      <c r="K164">
+      <c r="L164">
         <v>3280</v>
       </c>
-      <c r="L164">
+      <c r="M164">
         <v>2860</v>
       </c>
-      <c r="M164">
+      <c r="N164">
         <f t="shared" si="0"/>
         <v>12.850609756097562</v>
       </c>
-      <c r="N164">
+      <c r="O164">
         <f t="shared" si="1"/>
         <v>11.234265734265735</v>
       </c>
     </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>51</v>
       </c>
@@ -20785,22 +20804,22 @@
       <c r="J165">
         <v>42690</v>
       </c>
-      <c r="K165">
+      <c r="L165">
         <v>3320</v>
       </c>
-      <c r="L165">
+      <c r="M165">
         <v>2880</v>
       </c>
-      <c r="M165">
+      <c r="N165">
         <f t="shared" si="0"/>
         <v>12.858433734939759</v>
       </c>
-      <c r="N165">
+      <c r="O165">
         <f t="shared" si="1"/>
         <v>11.232638888888889</v>
       </c>
     </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>34</v>
       </c>
@@ -20816,22 +20835,22 @@
       <c r="J166">
         <v>43780</v>
       </c>
-      <c r="K166">
+      <c r="L166">
         <v>3410</v>
       </c>
-      <c r="L166">
+      <c r="M166">
         <v>2830</v>
       </c>
-      <c r="M166">
+      <c r="N166">
         <f t="shared" si="0"/>
         <v>12.838709677419354</v>
       </c>
-      <c r="N166">
+      <c r="O166">
         <f t="shared" si="1"/>
         <v>11.254416961130742</v>
       </c>
     </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>35</v>
       </c>
@@ -20847,22 +20866,22 @@
       <c r="J167">
         <v>42800</v>
       </c>
-      <c r="K167">
+      <c r="L167">
         <v>3330</v>
       </c>
-      <c r="L167">
+      <c r="M167">
         <v>2820</v>
       </c>
-      <c r="M167">
+      <c r="N167">
         <f t="shared" si="0"/>
         <v>12.852852852852854</v>
       </c>
-      <c r="N167">
+      <c r="O167">
         <f t="shared" si="1"/>
         <v>11.25531914893617</v>
       </c>
     </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>40</v>
       </c>
@@ -20878,22 +20897,22 @@
       <c r="J168">
         <v>53070</v>
       </c>
-      <c r="K168">
+      <c r="L168">
         <v>4130</v>
       </c>
-      <c r="L168">
+      <c r="M168">
         <v>2780</v>
       </c>
-      <c r="M168">
+      <c r="N168">
         <f t="shared" si="0"/>
         <v>12.849878934624698</v>
       </c>
-      <c r="N168">
+      <c r="O168">
         <f t="shared" si="1"/>
         <v>11.251798561151078</v>
       </c>
     </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>42</v>
       </c>
@@ -20909,22 +20928,22 @@
       <c r="J169">
         <v>44930</v>
       </c>
-      <c r="K169">
+      <c r="L169">
         <v>3500</v>
       </c>
-      <c r="L169">
+      <c r="M169">
         <v>2970</v>
       </c>
-      <c r="M169">
+      <c r="N169">
         <f t="shared" si="0"/>
         <v>12.837142857142856</v>
       </c>
-      <c r="N169">
+      <c r="O169">
         <f t="shared" si="1"/>
         <v>11.245791245791246</v>
       </c>
     </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>36</v>
       </c>
@@ -20940,22 +20959,22 @@
       <c r="J170">
         <v>45960</v>
       </c>
-      <c r="K170">
+      <c r="L170">
         <v>3580</v>
       </c>
-      <c r="L170">
+      <c r="M170">
         <v>2900</v>
       </c>
-      <c r="M170">
+      <c r="N170">
         <f t="shared" si="0"/>
         <v>12.837988826815643</v>
       </c>
-      <c r="N170">
+      <c r="O170">
         <f t="shared" si="1"/>
         <v>11.258620689655173</v>
       </c>
     </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>37</v>
       </c>
@@ -20971,22 +20990,22 @@
       <c r="J171">
         <v>46180</v>
       </c>
-      <c r="K171">
+      <c r="L171">
         <v>3590</v>
       </c>
-      <c r="L171">
+      <c r="M171">
         <v>2840</v>
       </c>
-      <c r="M171">
+      <c r="N171">
         <f t="shared" si="0"/>
         <v>12.863509749303621</v>
       </c>
-      <c r="N171">
+      <c r="O171">
         <f t="shared" si="1"/>
         <v>11.242957746478874</v>
       </c>
     </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>41</v>
       </c>
@@ -21002,22 +21021,22 @@
       <c r="J172">
         <v>50630</v>
       </c>
-      <c r="K172">
+      <c r="L172">
         <v>3940</v>
       </c>
-      <c r="L172">
+      <c r="M172">
         <v>2910</v>
       </c>
-      <c r="M172">
+      <c r="N172">
         <f t="shared" si="0"/>
         <v>12.850253807106599</v>
       </c>
-      <c r="N172">
+      <c r="O172">
         <f t="shared" si="1"/>
         <v>11.223367697594501</v>
       </c>
     </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>38</v>
       </c>
@@ -21033,22 +21052,22 @@
       <c r="J173">
         <v>42450</v>
       </c>
-      <c r="K173">
+      <c r="L173">
         <v>3160</v>
       </c>
-      <c r="L173">
+      <c r="M173">
         <v>2710</v>
       </c>
-      <c r="M173">
+      <c r="N173">
         <f t="shared" si="0"/>
         <v>13.433544303797468</v>
       </c>
-      <c r="N173">
+      <c r="O173">
         <f t="shared" si="1"/>
         <v>10.963099630996309</v>
       </c>
     </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>51</v>
       </c>
@@ -21064,22 +21083,22 @@
       <c r="J174">
         <v>43180</v>
       </c>
-      <c r="K174">
+      <c r="L174">
         <v>3330</v>
       </c>
-      <c r="L174">
+      <c r="M174">
         <v>2790</v>
       </c>
-      <c r="M174">
+      <c r="N174">
         <f t="shared" si="0"/>
         <v>12.966966966966966</v>
       </c>
-      <c r="N174">
+      <c r="O174">
         <f t="shared" si="1"/>
         <v>10.935483870967742</v>
       </c>
     </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>34</v>
       </c>
@@ -21095,22 +21114,22 @@
       <c r="J175">
         <v>42720</v>
       </c>
-      <c r="K175">
+      <c r="L175">
         <v>3410</v>
       </c>
-      <c r="L175">
+      <c r="M175">
         <v>2750</v>
       </c>
-      <c r="M175">
+      <c r="N175">
         <f t="shared" si="0"/>
         <v>12.527859237536656</v>
       </c>
-      <c r="N175">
+      <c r="O175">
         <f t="shared" si="1"/>
         <v>10.970909090909091</v>
       </c>
     </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>35</v>
       </c>
@@ -21126,22 +21145,22 @@
       <c r="J176">
         <v>41810</v>
       </c>
-      <c r="K176">
+      <c r="L176">
         <v>3350</v>
       </c>
-      <c r="L176">
+      <c r="M176">
         <v>2730</v>
       </c>
-      <c r="M176">
+      <c r="N176">
         <f t="shared" si="0"/>
         <v>12.480597014925372</v>
       </c>
-      <c r="N176">
+      <c r="O176">
         <f t="shared" si="1"/>
         <v>10.967032967032967</v>
       </c>
     </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>40</v>
       </c>
@@ -21157,22 +21176,22 @@
       <c r="J177">
         <v>49390</v>
       </c>
-      <c r="K177">
+      <c r="L177">
         <v>4080</v>
       </c>
-      <c r="L177">
+      <c r="M177">
         <v>2730</v>
       </c>
-      <c r="M177">
+      <c r="N177">
         <f t="shared" si="0"/>
         <v>12.105392156862745</v>
       </c>
-      <c r="N177">
+      <c r="O177">
         <f t="shared" si="1"/>
         <v>10.967032967032967</v>
       </c>
     </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>42</v>
       </c>
@@ -21188,22 +21207,22 @@
       <c r="J178">
         <v>44000</v>
       </c>
-      <c r="K178">
+      <c r="L178">
         <v>3430</v>
       </c>
-      <c r="L178">
+      <c r="M178">
         <v>2770</v>
       </c>
-      <c r="M178">
+      <c r="N178">
         <f t="shared" si="0"/>
         <v>12.827988338192419</v>
       </c>
-      <c r="N178">
+      <c r="O178">
         <f t="shared" si="1"/>
         <v>10.974729241877256</v>
       </c>
     </row>
-    <row r="179" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>36</v>
       </c>
@@ -21219,22 +21238,22 @@
       <c r="J179">
         <v>44910</v>
       </c>
-      <c r="K179">
+      <c r="L179">
         <v>3620</v>
       </c>
-      <c r="L179">
+      <c r="M179">
         <v>2790</v>
       </c>
-      <c r="M179">
+      <c r="N179">
         <f t="shared" si="0"/>
         <v>12.406077348066299</v>
       </c>
-      <c r="N179">
+      <c r="O179">
         <f t="shared" si="1"/>
         <v>10.978494623655914</v>
       </c>
     </row>
-    <row r="180" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>37</v>
       </c>
@@ -21250,22 +21269,22 @@
       <c r="J180">
         <v>44090</v>
       </c>
-      <c r="K180">
+      <c r="L180">
         <v>3460</v>
       </c>
-      <c r="L180">
+      <c r="M180">
         <v>2790</v>
       </c>
-      <c r="M180">
+      <c r="N180">
         <f t="shared" si="0"/>
         <v>12.742774566473988</v>
       </c>
-      <c r="N180">
+      <c r="O180">
         <f t="shared" si="1"/>
         <v>10.978494623655914</v>
       </c>
     </row>
-    <row r="181" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>41</v>
       </c>
@@ -21281,22 +21300,22 @@
       <c r="J181">
         <v>47010</v>
       </c>
-      <c r="K181">
+      <c r="L181">
         <v>3770</v>
       </c>
-      <c r="L181">
+      <c r="M181">
         <v>2830</v>
       </c>
-      <c r="M181">
+      <c r="N181">
         <f t="shared" si="0"/>
         <v>12.469496021220159</v>
       </c>
-      <c r="N181">
+      <c r="O181">
         <f t="shared" si="1"/>
         <v>10.943462897526501</v>
       </c>
     </row>
-    <row r="182" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>38</v>
       </c>
@@ -21312,22 +21331,22 @@
       <c r="J182">
         <v>40010</v>
       </c>
-      <c r="K182">
+      <c r="L182">
         <v>3020</v>
       </c>
-      <c r="L182">
+      <c r="M182">
         <v>2710</v>
       </c>
-      <c r="M182">
+      <c r="N182">
         <f t="shared" si="0"/>
         <v>13.248344370860927</v>
       </c>
-      <c r="N182">
+      <c r="O182">
         <f t="shared" si="1"/>
         <v>10.642066420664207</v>
       </c>
     </row>
-    <row r="183" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>51</v>
       </c>
@@ -21343,22 +21362,22 @@
       <c r="J183">
         <v>41420</v>
       </c>
-      <c r="K183">
+      <c r="L183">
         <v>3200</v>
       </c>
-      <c r="L183">
+      <c r="M183">
         <v>2800</v>
       </c>
-      <c r="M183">
+      <c r="N183">
         <f t="shared" si="0"/>
         <v>12.94375</v>
       </c>
-      <c r="N183">
+      <c r="O183">
         <f t="shared" si="1"/>
         <v>10.553571428571429</v>
       </c>
     </row>
-    <row r="184" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>34</v>
       </c>
@@ -21374,22 +21393,22 @@
       <c r="J184">
         <v>41310</v>
       </c>
-      <c r="K184">
+      <c r="L184">
         <v>3270</v>
       </c>
-      <c r="L184">
+      <c r="M184">
         <v>2770</v>
       </c>
-      <c r="M184">
+      <c r="N184">
         <f t="shared" si="0"/>
         <v>12.63302752293578</v>
       </c>
-      <c r="N184">
+      <c r="O184">
         <f t="shared" si="1"/>
         <v>10.530685920577618</v>
       </c>
     </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>35</v>
       </c>
@@ -21405,22 +21424,22 @@
       <c r="J185">
         <v>41520</v>
       </c>
-      <c r="K185">
+      <c r="L185">
         <v>3330</v>
       </c>
-      <c r="L185">
+      <c r="M185">
         <v>2810</v>
       </c>
-      <c r="M185">
+      <c r="N185">
         <f t="shared" si="0"/>
         <v>12.468468468468469</v>
       </c>
-      <c r="N185">
+      <c r="O185">
         <f t="shared" si="1"/>
         <v>10.718861209964412</v>
       </c>
     </row>
-    <row r="186" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>40</v>
       </c>
@@ -21436,22 +21455,22 @@
       <c r="J186">
         <v>50800</v>
       </c>
-      <c r="K186">
+      <c r="L186">
         <v>4180</v>
       </c>
-      <c r="L186">
+      <c r="M186">
         <v>2860</v>
       </c>
-      <c r="M186">
+      <c r="N186">
         <f t="shared" si="0"/>
         <v>12.153110047846891</v>
       </c>
-      <c r="N186">
+      <c r="O186">
         <f t="shared" si="1"/>
         <v>10.475524475524475</v>
       </c>
     </row>
-    <row r="187" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>42</v>
       </c>
@@ -21467,22 +21486,22 @@
       <c r="J187">
         <v>42470</v>
       </c>
-      <c r="K187">
+      <c r="L187">
         <v>3290</v>
       </c>
-      <c r="L187">
+      <c r="M187">
         <v>2890</v>
       </c>
-      <c r="M187">
+      <c r="N187">
         <f t="shared" si="0"/>
         <v>12.908814589665653</v>
       </c>
-      <c r="N187">
+      <c r="O187">
         <f t="shared" si="1"/>
         <v>10.570934256055363</v>
       </c>
     </row>
-    <row r="188" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>36</v>
       </c>
@@ -21498,22 +21517,22 @@
       <c r="J188">
         <v>44240</v>
       </c>
-      <c r="K188">
+      <c r="L188">
         <v>3480</v>
       </c>
-      <c r="L188">
+      <c r="M188">
         <v>2900</v>
       </c>
-      <c r="M188">
+      <c r="N188">
         <f t="shared" si="0"/>
         <v>12.712643678160919</v>
       </c>
-      <c r="N188">
+      <c r="O188">
         <f t="shared" si="1"/>
         <v>11.127586206896552</v>
       </c>
     </row>
-    <row r="189" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>37</v>
       </c>
@@ -21529,22 +21548,22 @@
       <c r="J189">
         <v>43650</v>
       </c>
-      <c r="K189">
+      <c r="L189">
         <v>3410</v>
       </c>
-      <c r="L189">
+      <c r="M189">
         <v>2840</v>
       </c>
-      <c r="M189">
+      <c r="N189">
         <f t="shared" si="0"/>
         <v>12.80058651026393</v>
       </c>
-      <c r="N189">
+      <c r="O189">
         <f t="shared" si="1"/>
         <v>11.05281690140845</v>
       </c>
     </row>
-    <row r="190" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>41</v>
       </c>
@@ -21560,22 +21579,22 @@
       <c r="J190">
         <v>46150</v>
       </c>
-      <c r="K190">
+      <c r="L190">
         <v>3660</v>
       </c>
-      <c r="L190">
+      <c r="M190">
         <v>2850</v>
       </c>
-      <c r="M190">
+      <c r="N190">
         <f t="shared" si="0"/>
         <v>12.609289617486338</v>
       </c>
-      <c r="N190">
+      <c r="O190">
         <f t="shared" si="1"/>
         <v>10.747368421052631</v>
       </c>
     </row>
-    <row r="191" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>38</v>
       </c>
@@ -21591,22 +21610,22 @@
       <c r="J191">
         <v>37010</v>
       </c>
-      <c r="K191">
+      <c r="L191">
         <v>2850</v>
       </c>
-      <c r="L191">
+      <c r="M191">
         <v>2520</v>
       </c>
-      <c r="M191">
+      <c r="N191">
         <f t="shared" si="0"/>
         <v>12.985964912280702</v>
       </c>
-      <c r="N191">
+      <c r="O191">
         <f t="shared" si="1"/>
         <v>9.4960317460317452</v>
       </c>
     </row>
-    <row r="192" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>51</v>
       </c>
@@ -21622,22 +21641,22 @@
       <c r="J192">
         <v>38960</v>
       </c>
-      <c r="K192">
+      <c r="L192">
         <v>3060</v>
       </c>
-      <c r="L192">
+      <c r="M192">
         <v>2710</v>
       </c>
-      <c r="M192">
+      <c r="N192">
         <f t="shared" si="0"/>
         <v>12.732026143790849</v>
       </c>
-      <c r="N192">
+      <c r="O192">
         <f t="shared" si="1"/>
         <v>8.8634686346863472</v>
       </c>
     </row>
-    <row r="193" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>34</v>
       </c>
@@ -21653,22 +21672,22 @@
       <c r="J193">
         <v>38740</v>
       </c>
-      <c r="K193">
+      <c r="L193">
         <v>3200</v>
       </c>
-      <c r="L193">
+      <c r="M193">
         <v>2610</v>
       </c>
-      <c r="M193">
+      <c r="N193">
         <f t="shared" si="0"/>
         <v>12.106249999999999</v>
       </c>
-      <c r="N193">
+      <c r="O193">
         <f t="shared" si="1"/>
         <v>9.3869731800766285</v>
       </c>
     </row>
-    <row r="194" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>35</v>
       </c>
@@ -21684,22 +21703,22 @@
       <c r="J194">
         <v>39950</v>
       </c>
-      <c r="K194">
+      <c r="L194">
         <v>3300</v>
       </c>
-      <c r="L194">
+      <c r="M194">
         <v>2550</v>
       </c>
-      <c r="M194">
+      <c r="N194">
         <f t="shared" si="0"/>
         <v>12.106060606060606</v>
       </c>
-      <c r="N194">
+      <c r="O194">
         <f t="shared" si="1"/>
         <v>9.7019607843137248</v>
       </c>
     </row>
-    <row r="195" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>40</v>
       </c>
@@ -21715,22 +21734,22 @@
       <c r="J195">
         <v>50180</v>
       </c>
-      <c r="K195">
+      <c r="L195">
         <v>4200</v>
       </c>
-      <c r="L195">
+      <c r="M195">
         <v>2600</v>
       </c>
-      <c r="M195">
+      <c r="N195">
         <f t="shared" si="0"/>
         <v>11.947619047619048</v>
       </c>
-      <c r="N195">
+      <c r="O195">
         <f t="shared" si="1"/>
         <v>9.3115384615384613</v>
       </c>
     </row>
-    <row r="196" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>42</v>
       </c>
@@ -21746,22 +21765,22 @@
       <c r="J196">
         <v>39650</v>
       </c>
-      <c r="K196">
+      <c r="L196">
         <v>3190</v>
       </c>
-      <c r="L196">
+      <c r="M196">
         <v>2650</v>
       </c>
-      <c r="M196">
+      <c r="N196">
         <f t="shared" si="0"/>
         <v>12.429467084639498</v>
       </c>
-      <c r="N196">
+      <c r="O196">
         <f t="shared" si="1"/>
         <v>9.4792452830188676</v>
       </c>
     </row>
-    <row r="197" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>36</v>
       </c>
@@ -21777,22 +21796,22 @@
       <c r="J197">
         <v>41360</v>
       </c>
-      <c r="K197">
+      <c r="L197">
         <v>3460</v>
       </c>
-      <c r="L197">
+      <c r="M197">
         <v>2650</v>
       </c>
-      <c r="M197">
+      <c r="N197">
         <f t="shared" si="0"/>
         <v>11.953757225433526</v>
       </c>
-      <c r="N197">
+      <c r="O197">
         <f t="shared" si="1"/>
         <v>9.8716981132075468</v>
       </c>
     </row>
-    <row r="198" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>37</v>
       </c>
@@ -21808,22 +21827,22 @@
       <c r="J198">
         <v>41900</v>
       </c>
-      <c r="K198">
+      <c r="L198">
         <v>3350</v>
       </c>
-      <c r="L198">
+      <c r="M198">
         <v>2640</v>
       </c>
-      <c r="M198">
+      <c r="N198">
         <f t="shared" si="0"/>
         <v>12.507462686567164</v>
       </c>
-      <c r="N198">
+      <c r="O198">
         <f t="shared" si="1"/>
         <v>9.9469696969696972</v>
       </c>
     </row>
-    <row r="199" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>41</v>
       </c>
@@ -21839,22 +21858,22 @@
       <c r="J199">
         <v>44490</v>
       </c>
-      <c r="K199">
+      <c r="L199">
         <v>3580</v>
       </c>
-      <c r="L199">
+      <c r="M199">
         <v>2710</v>
       </c>
-      <c r="M199">
+      <c r="N199">
         <f t="shared" si="0"/>
         <v>12.427374301675977</v>
       </c>
-      <c r="N199">
+      <c r="O199">
         <f t="shared" si="1"/>
         <v>9.6199261992619931</v>
       </c>
     </row>
-    <row r="200" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>57</v>
       </c>
@@ -21865,10 +21884,13 @@
         <v>34574</v>
       </c>
       <c r="G200">
-        <v>14546.1538461538</v>
-      </c>
-    </row>
-    <row r="201" spans="1:14" x14ac:dyDescent="0.3">
+        <v>14546.153849999999</v>
+      </c>
+      <c r="J200">
+        <v>39630.384619999997</v>
+      </c>
+    </row>
+    <row r="201" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>57</v>
       </c>
@@ -21879,10 +21901,13 @@
         <v>34999</v>
       </c>
       <c r="G201">
-        <v>14499.9999999999</v>
-      </c>
-    </row>
-    <row r="202" spans="1:14" x14ac:dyDescent="0.3">
+        <v>14500</v>
+      </c>
+      <c r="J201">
+        <v>38340.384619999997</v>
+      </c>
+    </row>
+    <row r="202" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>57</v>
       </c>
@@ -21893,10 +21918,13 @@
         <v>35152</v>
       </c>
       <c r="G202">
-        <v>14996.1538461538</v>
-      </c>
-    </row>
-    <row r="203" spans="1:14" x14ac:dyDescent="0.3">
+        <v>14996.153850000001</v>
+      </c>
+      <c r="J202">
+        <v>39242.692309999999</v>
+      </c>
+    </row>
+    <row r="203" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>57</v>
       </c>
@@ -21907,10 +21935,13 @@
         <v>35361</v>
       </c>
       <c r="G203">
-        <v>14315.384615384601</v>
-      </c>
-    </row>
-    <row r="204" spans="1:14" x14ac:dyDescent="0.3">
+        <v>14315.384619999999</v>
+      </c>
+      <c r="J203">
+        <v>38041.538460000003</v>
+      </c>
+    </row>
+    <row r="204" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>57</v>
       </c>
@@ -21921,10 +21952,13 @@
         <v>35514</v>
       </c>
       <c r="G204">
-        <v>14765.384615384599</v>
-      </c>
-    </row>
-    <row r="205" spans="1:14" x14ac:dyDescent="0.3">
+        <v>14765.384620000001</v>
+      </c>
+      <c r="J204">
+        <v>40433.461539999997</v>
+      </c>
+    </row>
+    <row r="205" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>57</v>
       </c>
@@ -21935,10 +21969,13 @@
         <v>35729</v>
       </c>
       <c r="G205">
-        <v>14511.538461538401</v>
-      </c>
-    </row>
-    <row r="206" spans="1:14" x14ac:dyDescent="0.3">
+        <v>14511.53846</v>
+      </c>
+      <c r="J205">
+        <v>41220.384619999997</v>
+      </c>
+    </row>
+    <row r="206" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>57</v>
       </c>
@@ -21949,10 +21986,13 @@
         <v>35910</v>
       </c>
       <c r="G206">
-        <v>15261.538461538401</v>
-      </c>
-    </row>
-    <row r="207" spans="1:14" x14ac:dyDescent="0.3">
+        <v>15261.53846</v>
+      </c>
+      <c r="J206">
+        <v>39241.538460000003</v>
+      </c>
+    </row>
+    <row r="207" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>57</v>
       </c>
@@ -21963,10 +22003,13 @@
         <v>36093</v>
       </c>
       <c r="G207">
-        <v>14753.8461538461</v>
-      </c>
-    </row>
-    <row r="208" spans="1:14" x14ac:dyDescent="0.3">
+        <v>14753.846149999999</v>
+      </c>
+      <c r="J207">
+        <v>39596.92308</v>
+      </c>
+    </row>
+    <row r="208" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>57</v>
       </c>
@@ -21979,8 +22022,11 @@
       <c r="G208">
         <v>15250</v>
       </c>
-    </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J208">
+        <v>39991.538460000003</v>
+      </c>
+    </row>
+    <row r="209" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>57</v>
       </c>
@@ -21991,10 +22037,13 @@
         <v>36461</v>
       </c>
       <c r="G209">
-        <v>14730.7692307692</v>
-      </c>
-    </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
+        <v>14730.76923</v>
+      </c>
+      <c r="J209">
+        <v>38495</v>
+      </c>
+    </row>
+    <row r="210" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>57</v>
       </c>
@@ -22005,7 +22054,446 @@
         <v>36642</v>
       </c>
       <c r="G210">
-        <v>14523.0769230769</v>
+        <v>14523.07692</v>
+      </c>
+      <c r="J210">
+        <v>38883.846149999998</v>
+      </c>
+    </row>
+    <row r="211" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>59</v>
+      </c>
+      <c r="B211" t="s">
+        <v>58</v>
+      </c>
+      <c r="F211" s="4">
+        <v>34574</v>
+      </c>
+      <c r="G211">
+        <v>14244.74187</v>
+      </c>
+      <c r="J211">
+        <v>38162.906309999998</v>
+      </c>
+    </row>
+    <row r="212" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
+        <v>59</v>
+      </c>
+      <c r="B212" t="s">
+        <v>58</v>
+      </c>
+      <c r="F212" s="4">
+        <v>34999</v>
+      </c>
+      <c r="G212">
+        <v>13739.96176</v>
+      </c>
+      <c r="J212">
+        <v>37796.940730000002</v>
+      </c>
+    </row>
+    <row r="213" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
+        <v>59</v>
+      </c>
+      <c r="B213" t="s">
+        <v>58</v>
+      </c>
+      <c r="F213" s="4">
+        <v>35152</v>
+      </c>
+      <c r="G213">
+        <v>14244.74187</v>
+      </c>
+      <c r="J213">
+        <v>37960.994259999999</v>
+      </c>
+    </row>
+    <row r="214" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A214" t="s">
+        <v>59</v>
+      </c>
+      <c r="B214" t="s">
+        <v>58</v>
+      </c>
+      <c r="F214" s="4">
+        <v>35361</v>
+      </c>
+      <c r="G214">
+        <v>13751.43403</v>
+      </c>
+      <c r="J214">
+        <v>38515.105159999999</v>
+      </c>
+    </row>
+    <row r="215" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A215" t="s">
+        <v>59</v>
+      </c>
+      <c r="B215" t="s">
+        <v>58</v>
+      </c>
+      <c r="F215" s="4">
+        <v>35514</v>
+      </c>
+      <c r="G215">
+        <v>13717.01721</v>
+      </c>
+      <c r="J215">
+        <v>39048.565970000003</v>
+      </c>
+    </row>
+    <row r="216" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A216" t="s">
+        <v>59</v>
+      </c>
+      <c r="B216" t="s">
+        <v>58</v>
+      </c>
+      <c r="F216" s="4">
+        <v>35729</v>
+      </c>
+      <c r="G216">
+        <v>13476.09943</v>
+      </c>
+      <c r="J216">
+        <v>38189.292540000002</v>
+      </c>
+    </row>
+    <row r="217" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
+        <v>59</v>
+      </c>
+      <c r="B217" t="s">
+        <v>58</v>
+      </c>
+      <c r="F217" s="4">
+        <v>35910</v>
+      </c>
+      <c r="G217">
+        <v>14485.659659999999</v>
+      </c>
+      <c r="J217">
+        <v>38429.063099999999</v>
+      </c>
+    </row>
+    <row r="218" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A218" t="s">
+        <v>59</v>
+      </c>
+      <c r="B218" t="s">
+        <v>58</v>
+      </c>
+      <c r="F218" s="4">
+        <v>36093</v>
+      </c>
+      <c r="G218">
+        <v>14497.13193</v>
+      </c>
+      <c r="J218">
+        <v>39424.856599999999</v>
+      </c>
+    </row>
+    <row r="219" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
+        <v>59</v>
+      </c>
+      <c r="B219" t="s">
+        <v>58</v>
+      </c>
+      <c r="F219" s="4">
+        <v>36307</v>
+      </c>
+      <c r="G219">
+        <v>16263.862329999998</v>
+      </c>
+      <c r="J219">
+        <v>41557.552580000003</v>
+      </c>
+    </row>
+    <row r="220" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A220" t="s">
+        <v>59</v>
+      </c>
+      <c r="B220" t="s">
+        <v>58</v>
+      </c>
+      <c r="F220" s="4">
+        <v>36461</v>
+      </c>
+      <c r="G220">
+        <v>15231.357550000001</v>
+      </c>
+      <c r="J220">
+        <v>40285.277249999999</v>
+      </c>
+    </row>
+    <row r="221" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A221" t="s">
+        <v>59</v>
+      </c>
+      <c r="B221" t="s">
+        <v>58</v>
+      </c>
+      <c r="F221" s="4">
+        <v>36642</v>
+      </c>
+      <c r="G221">
+        <v>15495.21989</v>
+      </c>
+      <c r="J221">
+        <v>40233.652009999998</v>
+      </c>
+    </row>
+    <row r="222" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A222" t="s">
+        <v>60</v>
+      </c>
+      <c r="B222" t="s">
+        <v>61</v>
+      </c>
+      <c r="F222" s="3">
+        <v>29936</v>
+      </c>
+      <c r="G222">
+        <v>37315.199999999997</v>
+      </c>
+      <c r="J222">
+        <v>63294.400000000001</v>
+      </c>
+      <c r="K222">
+        <v>2929.363636</v>
+      </c>
+      <c r="L222">
+        <v>5146.363636</v>
+      </c>
+    </row>
+    <row r="223" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A223" t="s">
+        <v>60</v>
+      </c>
+      <c r="B223" t="s">
+        <v>61</v>
+      </c>
+      <c r="F223" s="3">
+        <v>30292</v>
+      </c>
+      <c r="G223">
+        <v>34086</v>
+      </c>
+      <c r="K223">
+        <v>2653.74</v>
+      </c>
+    </row>
+    <row r="224" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A224" t="s">
+        <v>60</v>
+      </c>
+      <c r="B224" t="s">
+        <v>61</v>
+      </c>
+      <c r="F224" s="3">
+        <v>30560</v>
+      </c>
+      <c r="G224">
+        <v>30579.545450000001</v>
+      </c>
+      <c r="J224">
+        <v>55942.545449999998</v>
+      </c>
+      <c r="K224">
+        <v>2128.963636</v>
+      </c>
+      <c r="L224">
+        <v>4045.363636</v>
+      </c>
+    </row>
+    <row r="225" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A225" t="s">
+        <v>60</v>
+      </c>
+      <c r="B225" t="s">
+        <v>61</v>
+      </c>
+      <c r="F225" s="3">
+        <v>30957</v>
+      </c>
+      <c r="G225">
+        <v>30623.58</v>
+      </c>
+      <c r="K225">
+        <v>2189.5079999999998</v>
+      </c>
+    </row>
+    <row r="226" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A226" t="s">
+        <v>60</v>
+      </c>
+      <c r="B226" t="s">
+        <v>61</v>
+      </c>
+      <c r="F226" s="3">
+        <v>31319</v>
+      </c>
+      <c r="G226">
+        <v>30155.50909</v>
+      </c>
+      <c r="J226">
+        <v>59166.309090000002</v>
+      </c>
+      <c r="K226">
+        <v>2067.4909090000001</v>
+      </c>
+      <c r="L226">
+        <v>4348.2909090000003</v>
+      </c>
+    </row>
+    <row r="227" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A227" t="s">
+        <v>60</v>
+      </c>
+      <c r="B227" t="s">
+        <v>61</v>
+      </c>
+      <c r="F227" s="3">
+        <v>31783</v>
+      </c>
+      <c r="G227">
+        <v>27214.98</v>
+      </c>
+    </row>
+    <row r="228" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A228" t="s">
+        <v>60</v>
+      </c>
+      <c r="B228" t="s">
+        <v>61</v>
+      </c>
+      <c r="F228" s="3">
+        <v>32080</v>
+      </c>
+      <c r="G228">
+        <v>27497.127270000001</v>
+      </c>
+      <c r="J228">
+        <v>50433.027269999999</v>
+      </c>
+      <c r="K228">
+        <v>1935.3872730000001</v>
+      </c>
+      <c r="L228">
+        <v>3447.3872729999998</v>
+      </c>
+    </row>
+    <row r="229" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A229" t="s">
+        <v>60</v>
+      </c>
+      <c r="B229" t="s">
+        <v>61</v>
+      </c>
+      <c r="F229" s="3">
+        <v>33186</v>
+      </c>
+      <c r="G229">
+        <v>22229.29091</v>
+      </c>
+      <c r="J229">
+        <v>46053.090909999999</v>
+      </c>
+      <c r="K229">
+        <v>1242</v>
+      </c>
+      <c r="L229">
+        <v>2754</v>
+      </c>
+    </row>
+    <row r="230" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A230" t="s">
+        <v>60</v>
+      </c>
+      <c r="B230" t="s">
+        <v>61</v>
+      </c>
+      <c r="F230" s="3">
+        <v>34367</v>
+      </c>
+      <c r="G230">
+        <v>23322</v>
+      </c>
+      <c r="J230">
+        <v>53872</v>
+      </c>
+      <c r="K230">
+        <v>1035</v>
+      </c>
+      <c r="L230">
+        <v>2374</v>
+      </c>
+    </row>
+    <row r="231" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A231" t="s">
+        <v>60</v>
+      </c>
+      <c r="B231" t="s">
+        <v>61</v>
+      </c>
+      <c r="F231" s="3">
+        <v>35445</v>
+      </c>
+      <c r="G231">
+        <v>25322.966079999998</v>
+      </c>
+      <c r="J231">
+        <v>42968.287129999997</v>
+      </c>
+    </row>
+    <row r="232" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A232" t="s">
+        <v>60</v>
+      </c>
+      <c r="B232" t="s">
+        <v>61</v>
+      </c>
+      <c r="F232" s="3">
+        <v>36658</v>
+      </c>
+      <c r="G232">
+        <v>16594.5</v>
+      </c>
+      <c r="J232">
+        <v>34901.1</v>
+      </c>
+      <c r="K232">
+        <v>1224.2670000000001</v>
+      </c>
+      <c r="L232">
+        <v>2707.0857999999998</v>
+      </c>
+    </row>
+    <row r="233" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A233" t="s">
+        <v>60</v>
+      </c>
+      <c r="B233" t="s">
+        <v>61</v>
+      </c>
+      <c r="F233" s="3">
+        <v>37928</v>
+      </c>
+      <c r="G233">
+        <v>22963.200000000001</v>
+      </c>
+      <c r="J233">
+        <v>59670</v>
+      </c>
+      <c r="K233">
+        <v>1242</v>
+      </c>
+      <c r="L233">
+        <v>2754</v>
       </c>
     </row>
   </sheetData>

</xml_diff>